<commit_message>
update class diagram for asp and updated product backlog
</commit_message>
<xml_diff>
--- a/documentation/productBacklog/Product Backlog.xlsx
+++ b/documentation/productBacklog/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Captsone\Group3Spring2024Capstone\documentation\productBacklog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BCAA1BF-2A6C-4B94-9EF7-1FA2254F096D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861368F0-6377-46EF-91C8-BD1330FA3DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1425" yWindow="1740" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="129" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +496,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
new backlog and updated wireframes
I updated the wireframes and ERD diagram because they need to match upcoming changes to the system

-Corey Williams
</commit_message>
<xml_diff>
--- a/documentation/productBacklog/Product Backlog.xlsx
+++ b/documentation/productBacklog/Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Captsone\Group3Spring2024Capstone\documentation\productBacklog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{861368F0-6377-46EF-91C8-BD1330FA3DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559F4CA4-8C1F-4CA6-AE50-3A9E7BCA2471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="1740" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-11460" yWindow="-21600" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>As a…</t>
   </si>
@@ -119,6 +119,15 @@
   </si>
   <si>
     <t>Upload a pdf source</t>
+  </si>
+  <si>
+    <t>Upload a hosted pdf source</t>
+  </si>
+  <si>
+    <t>Build Project</t>
+  </si>
+  <si>
+    <t>I can group a set of sources while working on project</t>
   </si>
 </sst>
 </file>
@@ -465,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="129" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +505,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
@@ -510,7 +519,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>
@@ -524,7 +533,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
@@ -552,58 +561,58 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -614,24 +623,24 @@
         <v>4</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -642,29 +651,57 @@
         <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>10</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D13">
-    <sortCondition ref="A2:A13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D15">
+    <sortCondition ref="A2:A15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added missing product backlog and fixed docstrings
added missing backlogs with the updated for this sprint's goals and updated docstrings to increase documentation

-Corey WIlliams
</commit_message>
<xml_diff>
--- a/documentation/productBacklog/Product Backlog.xlsx
+++ b/documentation/productBacklog/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Captsone\Group3Spring2024Capstone\documentation\productBacklog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559F4CA4-8C1F-4CA6-AE50-3A9E7BCA2471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1450A529-603E-4782-95D4-84ABA849AB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11460" yWindow="-21600" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -477,7 +477,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,7 +575,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>4</v>
@@ -589,7 +589,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>4</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
@@ -687,7 +687,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>4</v>

</xml_diff>